<commit_message>
Grafana and prometheus (#4)
* WIP: migrate content (partial import)

* WIP: continue migration

* .bashrc alias update

* WIP:  ArgoCD

* WIP

* wip

* WIP

* WIP

* WIP

* WIP

* WIP

* WIP

* ArgoCD - working with tweaks and no 2nd cluster yet

* Finish:  ArgoCD automation

* ArgoCD - removed secrets

* WIP:  grafana and prometheous

* WIP:  grafana-prometheus

* WIP:  grafana

* WIP:  grafana

* grafana:  complete
</commit_message>
<xml_diff>
--- a/users/Bryan/linux k8s vim cheat sheet.xlsx
+++ b/users/Bryan/linux k8s vim cheat sheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="196">
   <si>
     <t xml:space="preserve">rmdir foldername</t>
   </si>
@@ -649,12 +649,15 @@
     <t xml:space="preserve">kubectl get pod &lt;pod-name&gt; -n &lt;namespace&gt; -o yaml</t>
   </si>
   <si>
+    <t xml:space="preserve">kubectl delete -n argocd -f https://raw.githubusercontent.com/argoproj/argo-cd/stable/manifests/install.yaml
+kubectl delete namespace argocd</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
         <u val="single"/>
         <sz val="11"/>
-        <color indexed="64"/>
         <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">Search And Replace
@@ -663,7 +666,6 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="64"/>
         <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">
@@ -679,12 +681,27 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">kubectl logs -n monitoring deployment/monitoring-grafana | grep -i dashboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check logs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shift V
+"+y
+d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select lines 
+yank to clipboard
+delete</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
         <u val="single"/>
         <sz val="11"/>
-        <color indexed="64"/>
         <rFont val="Aptos Narrow"/>
         <scheme val="minor"/>
       </rPr>
@@ -695,7 +712,6 @@
       <rPr>
         <u val="single"/>
         <sz val="11"/>
-        <color indexed="64"/>
         <rFont val="Aptos Narrow"/>
         <scheme val="minor"/>
       </rPr>
@@ -705,7 +721,6 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color indexed="64"/>
         <rFont val="Aptos Narrow"/>
         <scheme val="minor"/>
       </rPr>
@@ -715,16 +730,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">shift V
-"+y
-d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select lines 
-yank to clipboard
-delete</t>
-  </si>
-  <si>
     <t xml:space="preserve"># Test DNS resolution from within the ArgoCD namespace
 kubectl -n argocd run test-dns --image=busybox --rm -it --restart=Never -- nslookup BSUS103KM01</t>
   </si>
@@ -735,6 +740,15 @@
     <t xml:space="preserve">kubectl get pods -A -o custom-columns='NAMESPACE:.metadata.namespace,NAME:.metadata.name,CONTROLLER_KIND:.metadata.ownerReferences[0].kind,CONTROLLER_NAME:.metadata.ownerReferences[0].name' --sort-by=.metadata.namespace</t>
   </si>
   <si>
+    <t xml:space="preserve">Kubernetes apps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">helm show values prometheus-community/kube-prometheus-stack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">show what is configurable in a helm chart</t>
+  </si>
+  <si>
     <t>logs</t>
   </si>
   <si>
@@ -747,30 +761,19 @@
     <t>comment</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Asana"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">sudo </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <rFont val="Asana"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>mkdir</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Asana"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> -p /srv/secrets/{ssh-keys,clusters}</t>
-    </r>
+    <t xml:space="preserve">mv /path/to/source/* /path/to/destination/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">move everything</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mv file1.txt file2.txt /path/to/destination/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">move some things</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mkdir -p /srv/secrets/{ssh-keys,clusters}</t>
   </si>
   <si>
     <t xml:space="preserve">sudo chgrp -R gitadmins /path/to/dir</t>
@@ -807,7 +810,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -856,20 +859,24 @@
     </font>
     <font>
       <sz val="11.000000"/>
-      <color indexed="64"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
       <u/>
       <sz val="11.000000"/>
-      <color indexed="64"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.000000"/>
-      <name val="Asana"/>
+      <sz val="12.000000"/>
+      <color indexed="64"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12.000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -892,7 +899,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -940,14 +947,20 @@
     <xf fontId="7" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="3" vertical="center" wrapText="1"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="8" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf fontId="9" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="10" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1000,8 +1013,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" displayName="Table7" ref="D1:E12">
-  <autoFilter ref="D1:E12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" displayName="Table7" ref="D1:E13">
+  <autoFilter ref="D1:E13"/>
   <tableColumns count="2">
     <tableColumn id="1" name="kubernetes"/>
     <tableColumn id="2" name="comments"/>
@@ -1011,8 +1024,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" displayName="Table1" ref="A24:B29">
-  <autoFilter ref="A24:B29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" displayName="Table1" ref="A24:B31">
+  <autoFilter ref="A24:B31"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Linux"/>
     <tableColumn id="2" name="comment"/>
@@ -2224,7 +2237,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="100" workbookViewId="0">
       <selection activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -2233,8 +2246,7 @@
     <col customWidth="1" min="1" max="1" width="42.625"/>
     <col customWidth="1" min="2" max="2" width="33"/>
     <col customWidth="1" min="3" max="3" width="5.28515625"/>
-    <col customWidth="1" min="4" max="4" width="41.85546875"/>
-    <col customWidth="1" min="5" max="5" width="45.5703125"/>
+    <col customWidth="1" min="4" max="5" width="72.75390625"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75">
@@ -2275,12 +2287,15 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" ht="42.75">
       <c r="A5" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>39</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="6">
@@ -2313,35 +2328,38 @@
     </row>
     <row r="9" ht="99.75">
       <c r="A9" s="17" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>165</v>
+        <v>166</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="10" ht="57.75" customHeight="1">
       <c r="A10" s="7" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="11" ht="28.5">
+        <v>169</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" ht="42.75">
       <c r="A11" s="7" t="s">
         <v>55</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D11" t="s">
-        <v>169</v>
+      <c r="D11" s="9" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="12" ht="85.5">
@@ -2351,16 +2369,19 @@
       <c r="B12" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="9" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="13">
+      <c r="D12" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" ht="57">
       <c r="A13" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>46</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="14">
@@ -2368,17 +2389,23 @@
         <v>31</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="D14" s="8"/>
     </row>
     <row r="15">
-      <c r="D15" s="9"/>
-    </row>
-    <row r="16">
-      <c r="D16" s="9"/>
+      <c r="D15" s="8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" ht="15">
+      <c r="D16" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="E16" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="17" ht="16.5">
       <c r="A17" s="16" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="B17" t="s">
         <v>161</v>
@@ -2414,65 +2441,82 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>172</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="D21" s="9"/>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B24" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="25" ht="16.5">
-      <c r="A25" s="20" t="s">
-        <v>175</v>
-      </c>
-      <c r="B25" s="21"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" t="s">
-        <v>176</v>
-      </c>
-      <c r="B26" s="22" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>178</v>
-      </c>
-      <c r="B27" s="22" t="s">
-        <v>179</v>
-      </c>
+      <c r="A26" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="27" ht="15">
+      <c r="A27" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="B27" s="23"/>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="29" ht="18" customHeight="1">
-      <c r="A29" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="B29" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="31"/>
-    <row r="32"/>
-    <row r="33" ht="14.25">
-      <c r="A33" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="34" ht="14.25">
-      <c r="A34" t="s">
-        <v>184</v>
-      </c>
-      <c r="B34" t="s">
-        <v>185</v>
+        <v>186</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>188</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="31" ht="18" customHeight="1">
+      <c r="A31" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="B31" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35" ht="14.25">
+      <c r="A35" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="36" ht="14.25">
+      <c r="A36" t="s">
+        <v>194</v>
+      </c>
+      <c r="B36" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>